<commit_message>
Manejo de archivo de configuracio
</commit_message>
<xml_diff>
--- a/Excel/StockProductos.xlsx
+++ b/Excel/StockProductos.xlsx
@@ -10,15 +10,13 @@
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="PARACETAMOL 400 TABL" sheetId="2" r:id="rId2"/>
     <sheet name="PARACETAMOL 400 CAJA" sheetId="3" r:id="rId3"/>
-    <sheet name="IBUPROFENO 600 CAJA " sheetId="4" r:id="rId4"/>
-    <sheet name="IBUPROFENO 600 TABLE" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Producto</t>
   </si>
@@ -32,22 +30,13 @@
     <t>PARACETAMOL 400 CAJA CAPSULAS BLANDAS</t>
   </si>
   <si>
-    <t>IBUPROFENO 600 CAJA CAPSULAS BLANDAS</t>
-  </si>
-  <si>
-    <t>IBUPROFENO 600 TABLETA CAPSULAS BLANDAS</t>
-  </si>
-  <si>
     <t>Lote</t>
   </si>
   <si>
-    <t>f4</t>
+    <t>1a1a1a</t>
   </si>
   <si>
-    <t>g14</t>
-  </si>
-  <si>
-    <t>f3</t>
+    <t>1b1b1b</t>
   </si>
 </sst>
 </file>
@@ -119,40 +108,28 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>General!$A$2:$A$5</c:f>
+              <c:f>General!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>PARACETAMOL 400 TABLETA CAPSULAS BLANDAS</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>PARACETAMOL 400 CAJA CAPSULAS BLANDAS</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>IBUPROFENO 600 CAJA CAPSULAS BLANDAS</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>IBUPROFENO 600 TABLETA CAPSULAS BLANDAS</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>General!$B$2:$B$5</c:f>
+              <c:f>General!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>119</c:v>
-                </c:pt>
-                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -245,23 +222,29 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'PARACETAMOL 400 TABL'!$A$2:$A$2</c:f>
+              <c:f>'PARACETAMOL 400 TABL'!$A$2:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>f4</c:v>
+                  <c:v>1a1a1a</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1b1b1b</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'PARACETAMOL 400 TABL'!$B$2:$B$2</c:f>
+              <c:f>'PARACETAMOL 400 TABL'!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>56</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -357,7 +340,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>f4</c:v>
+                  <c:v>1a1a1a</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -369,7 +352,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -447,228 +430,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'IBUPROFENO 600 CAJA '!$A$2:$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>g14</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>f3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'IBUPROFENO 600 CAJA '!$B$2:$B$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>19</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50040001"/>
-        <c:axId val="50040002"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="50040001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Lotes</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr i="1" baseline="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="50040002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50040002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50040001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'IBUPROFENO 600 TABLE'!$A$2:$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>f3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'IBUPROFENO 600 TABLE'!$B$2:$B$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50050001"/>
-        <c:axId val="50050002"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="50050001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Lotes</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr i="1" baseline="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="50050002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50050002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50050001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -740,76 +501,6 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1129,7 +820,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1152,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>56</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1160,22 +851,6 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
         <v>0</v>
       </c>
     </row>
@@ -1187,7 +862,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1199,7 +874,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1207,10 +882,18 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>56</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1233,7 +916,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1241,83 +924,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>

</xml_diff>